<commit_message>
Add reagent transfer module (accessed from main menu))
</commit_message>
<xml_diff>
--- a/user_files/reagent_index.xlsx
+++ b/user_files/reagent_index.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="86">
   <si>
     <t>CAS-NO</t>
   </si>
@@ -443,6 +443,14 @@
       </rPr>
       <t>rine</t>
     </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diphenyl-sulfide</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thioxanen-9-one</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1367,8 +1375,8 @@
   </sheetPr>
   <dimension ref="A1:CG103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
@@ -2667,7 +2675,7 @@
       <c r="AM15"/>
     </row>
     <row r="16" spans="1:85" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="18" t="s">
         <v>54</v>
       </c>
       <c r="B16" s="11"/>
@@ -3024,7 +3032,9 @@
       <c r="AM22"/>
     </row>
     <row r="23" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
         <v>8</v>
@@ -3036,7 +3046,7 @@
         <v>65</v>
       </c>
       <c r="F23" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="G23"/>
       <c r="H23"/>
@@ -4305,7 +4315,9 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="16"/>
+      <c r="A51" s="16" t="s">
+        <v>84</v>
+      </c>
       <c r="B51" s="13"/>
       <c r="C51" s="13" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
work for 2nd gen model
</commit_message>
<xml_diff>
--- a/user_files/reagent_index.xlsx
+++ b/user_files/reagent_index.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2213" yWindow="1413" windowWidth="28800" windowHeight="18653"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="23233" windowHeight="12553"/>
   </bookViews>
   <sheets>
     <sheet name="reagent_index" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="94">
   <si>
     <t>CAS-NO</t>
   </si>
@@ -52,16 +52,9 @@
     <t>plate_5mL:001</t>
   </si>
   <si>
-    <t>plate_40mL:001</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>A3</t>
   </si>
   <si>
-    <t>plate_5mL:003</t>
-  </si>
-  <si>
     <t>A4</t>
   </si>
   <si>
@@ -140,10 +133,6 @@
     <t>D7</t>
   </si>
   <si>
-    <t>plate_40mL:003</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>A1</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -184,10 +173,6 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>plate_40mL:001</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>B3</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -239,10 +224,6 @@
   </si>
   <si>
     <t>plate_5mL:002</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>plate_5mL:003</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
@@ -268,22 +249,6 @@
   <si>
     <r>
       <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>plate_40mL:00</t>
     </r>
     <r>
       <rPr>
@@ -451,6 +416,180 @@
   </si>
   <si>
     <t>Thioxanen-9-one</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_50mL:001</t>
+  </si>
+  <si>
+    <t>plate_50mL:002</t>
+  </si>
+  <si>
+    <t>plate_50mL:003</t>
+  </si>
+  <si>
+    <t>KF</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>CsF</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>plate_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mL:00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>plate_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mL:001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>A4</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>B4</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>C4</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>est</t>
+    </r>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -995,7 +1134,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="11"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1015,6 +1154,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="19" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="8" xfId="36" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="28" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1375,8 +1515,8 @@
   </sheetPr>
   <dimension ref="A1:CG103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
@@ -1401,13 +1541,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -1495,10 +1635,10 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>6</v>
@@ -1588,14 +1728,14 @@
     </row>
     <row r="3" spans="1:85" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>6</v>
@@ -1685,14 +1825,14 @@
     </row>
     <row r="4" spans="1:85" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>6</v>
@@ -1782,14 +1922,14 @@
     </row>
     <row r="5" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>6</v>
@@ -1879,14 +2019,14 @@
     </row>
     <row r="6" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>6</v>
@@ -1976,14 +2116,14 @@
     </row>
     <row r="7" spans="1:85" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>6</v>
@@ -1994,14 +2134,14 @@
     </row>
     <row r="8" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>6</v>
@@ -2091,14 +2231,14 @@
     </row>
     <row r="9" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>6</v>
@@ -2188,14 +2328,14 @@
     </row>
     <row r="10" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>6</v>
@@ -2285,14 +2425,14 @@
     </row>
     <row r="11" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>6</v>
@@ -2382,14 +2522,14 @@
     </row>
     <row r="12" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>6</v>
@@ -2479,14 +2619,14 @@
     </row>
     <row r="13" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>6</v>
@@ -2578,7 +2718,7 @@
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>4</v>
@@ -2625,14 +2765,14 @@
     </row>
     <row r="15" spans="1:85" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>7</v>
@@ -2676,14 +2816,14 @@
     </row>
     <row r="16" spans="1:85" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>7</v>
@@ -2727,14 +2867,14 @@
     </row>
     <row r="17" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>7</v>
@@ -2778,14 +2918,14 @@
     </row>
     <row r="18" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>7</v>
@@ -2829,14 +2969,14 @@
     </row>
     <row r="19" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>7</v>
@@ -2880,17 +3020,17 @@
     </row>
     <row r="20" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F20" s="4">
         <v>0.1</v>
@@ -2931,17 +3071,17 @@
     </row>
     <row r="21" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F21" s="4">
         <v>8.5000000000000006E-2</v>
@@ -2982,17 +3122,17 @@
     </row>
     <row r="22" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F22" s="4">
         <v>7.0000000000000007E-2</v>
@@ -3033,17 +3173,17 @@
     </row>
     <row r="23" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F23" s="4">
         <v>6.0000000000000001E-3</v>
@@ -3083,16 +3223,18 @@
       <c r="AM23"/>
     </row>
     <row r="24" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="5"/>
+      <c r="A24" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F24" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3138,10 +3280,10 @@
         <v>8</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F25" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3182,17 +3324,17 @@
     </row>
     <row r="26" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="F26" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3238,10 +3380,10 @@
         <v>8</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F27" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3287,10 +3429,10 @@
         <v>8</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F28" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3336,10 +3478,10 @@
         <v>8</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F29" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3385,10 +3527,10 @@
         <v>8</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F30" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3434,10 +3576,10 @@
         <v>8</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F31" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3483,10 +3625,10 @@
         <v>8</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F32" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3532,10 +3674,10 @@
         <v>8</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F33" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3581,10 +3723,10 @@
         <v>8</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F34" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3630,10 +3772,10 @@
         <v>8</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F35" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3679,10 +3821,10 @@
         <v>8</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F36" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3728,10 +3870,10 @@
         <v>8</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F37" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3777,10 +3919,10 @@
         <v>8</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F38" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3826,10 +3968,10 @@
         <v>8</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F39" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3875,10 +4017,10 @@
         <v>8</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F40" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3924,10 +4066,10 @@
         <v>8</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F41" s="4">
         <v>5.0000000000000001E-3</v>
@@ -3973,10 +4115,10 @@
         <v>8</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F42" s="4">
         <v>5.0000000000000001E-3</v>
@@ -4022,10 +4164,10 @@
         <v>8</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F43" s="4">
         <v>5.0000000000000001E-3</v>
@@ -4071,10 +4213,10 @@
         <v>8</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F44" s="4">
         <v>5.0000000000000001E-3</v>
@@ -4120,10 +4262,10 @@
         <v>8</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F45" s="4">
         <v>5.0000000000000001E-3</v>
@@ -4169,10 +4311,10 @@
         <v>8</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F46" s="4">
         <v>5.0000000000000001E-3</v>
@@ -4212,16 +4354,18 @@
       <c r="AM46"/>
     </row>
     <row r="47" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="5"/>
+      <c r="A47" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F47" s="4">
         <v>5.0000000000000001E-3</v>
@@ -4262,11 +4406,11 @@
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A48" s="13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B48" s="13"/>
       <c r="C48" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D48" s="13" t="s">
         <v>4</v>
@@ -4280,14 +4424,14 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B49" s="13"/>
       <c r="C49" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>6</v>
@@ -4298,14 +4442,14 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B50" s="13"/>
       <c r="C50" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>6</v>
@@ -4316,14 +4460,14 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="16" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B51" s="13"/>
       <c r="C51" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>6</v>
@@ -4334,14 +4478,14 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="16" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B52" s="13"/>
       <c r="C52" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>6</v>
@@ -4352,14 +4496,14 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>6</v>
@@ -4370,14 +4514,14 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B54" s="13"/>
       <c r="C54" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E54" s="13" t="s">
         <v>6</v>
@@ -4388,14 +4532,14 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B55" s="13"/>
       <c r="C55" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E55" s="13" t="s">
         <v>6</v>
@@ -4408,10 +4552,10 @@
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E56" s="13" t="s">
         <v>6</v>
@@ -4424,10 +4568,10 @@
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E57" s="13" t="s">
         <v>6</v>
@@ -4440,10 +4584,10 @@
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E58" s="13" t="s">
         <v>6</v>
@@ -4456,10 +4600,10 @@
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E59" s="13" t="s">
         <v>6</v>
@@ -4472,10 +4616,10 @@
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E60" s="13" t="s">
         <v>6</v>
@@ -4488,10 +4632,10 @@
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E61" s="13" t="s">
         <v>6</v>
@@ -4504,10 +4648,10 @@
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E62" s="13" t="s">
         <v>6</v>
@@ -4520,10 +4664,10 @@
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D63" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E63" s="13" t="s">
         <v>6</v>
@@ -4536,10 +4680,10 @@
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" s="13" t="s">
         <v>58</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="E64" s="13" t="s">
         <v>6</v>
@@ -4552,10 +4696,10 @@
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>6</v>
@@ -4568,10 +4712,10 @@
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>6</v>
@@ -4584,10 +4728,10 @@
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E67" s="13" t="s">
         <v>6</v>
@@ -4600,10 +4744,10 @@
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E68" s="13" t="s">
         <v>6</v>
@@ -4616,10 +4760,10 @@
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E69" s="13" t="s">
         <v>6</v>
@@ -4632,10 +4776,10 @@
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E70" s="13" t="s">
         <v>6</v>
@@ -4648,10 +4792,10 @@
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E71" s="13" t="s">
         <v>6</v>
@@ -4664,10 +4808,10 @@
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E72" s="13" t="s">
         <v>6</v>
@@ -4680,10 +4824,10 @@
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E73" s="13" t="s">
         <v>6</v>
@@ -4696,10 +4840,10 @@
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E74" s="13" t="s">
         <v>6</v>
@@ -4712,10 +4856,10 @@
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E75" s="13" t="s">
         <v>6</v>
@@ -4727,8 +4871,8 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="14"/>
       <c r="B76" s="14"/>
-      <c r="C76" s="14" t="s">
-        <v>64</v>
+      <c r="C76" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="D76" s="14" t="s">
         <v>4</v>
@@ -4737,440 +4881,314 @@
         <v>6</v>
       </c>
       <c r="F76" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="14"/>
       <c r="B77" s="14"/>
-      <c r="C77" s="14" t="s">
-        <v>64</v>
+      <c r="C77" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E77" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F77" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
-      <c r="C78" s="14" t="s">
-        <v>11</v>
+      <c r="C78" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E78" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F78" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="14"/>
       <c r="B79" s="14"/>
-      <c r="C79" s="14" t="s">
-        <v>11</v>
+      <c r="C79" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E79" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F79" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="14"/>
       <c r="B80" s="14"/>
-      <c r="C80" s="14" t="s">
-        <v>11</v>
+      <c r="C80" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E80" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F80" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="14"/>
       <c r="B81" s="14"/>
-      <c r="C81" s="14" t="s">
-        <v>11</v>
+      <c r="C81" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E81" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F81" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="14"/>
       <c r="B82" s="14"/>
-      <c r="C82" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D82" s="14" t="s">
-        <v>60</v>
+      <c r="C82" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="E82" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F82" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
-      <c r="C83" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>61</v>
+      <c r="C83" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="E83" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F83" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
-      <c r="C84" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>10</v>
+      <c r="C84" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="E84" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F84" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="14"/>
       <c r="B85" s="14"/>
-      <c r="C85" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>23</v>
+      <c r="C85" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D85" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="E85" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F85" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="14"/>
       <c r="B86" s="14"/>
-      <c r="C86" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>24</v>
+      <c r="C86" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D86" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="E86" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F86" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A87" s="14"/>
+      <c r="A87" s="19" t="s">
+        <v>93</v>
+      </c>
       <c r="B87" s="14"/>
-      <c r="C87" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>25</v>
+      <c r="C87" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D87" s="19" t="s">
+        <v>92</v>
       </c>
       <c r="E87" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F87" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="14"/>
       <c r="B88" s="14"/>
-      <c r="C88" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E88" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F88" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C88" s="19"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="14"/>
       <c r="B89" s="14"/>
-      <c r="C89" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E89" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F89" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="14"/>
       <c r="B90" s="14"/>
-      <c r="C90" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E90" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F90" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="14"/>
       <c r="B91" s="14"/>
-      <c r="C91" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E91" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F91" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="14"/>
       <c r="B92" s="14"/>
-      <c r="C92" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E92" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F92" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="14"/>
       <c r="B93" s="14"/>
-      <c r="C93" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E93" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F93" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="14"/>
       <c r="B94" s="14"/>
-      <c r="C94" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E94" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F94" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="14"/>
       <c r="B95" s="14"/>
-      <c r="C95" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E95" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F95" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="14"/>
       <c r="B96" s="14"/>
-      <c r="C96" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E96" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F96" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="14"/>
       <c r="B97" s="14"/>
-      <c r="C97" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D97" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E97" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F97" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="14"/>
       <c r="B98" s="14"/>
-      <c r="C98" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E98" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F98" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="14"/>
       <c r="B99" s="14"/>
-      <c r="C99" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D99" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E99" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F99" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="14"/>
       <c r="B100" s="14"/>
-      <c r="C100" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E100" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F100" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="14"/>
       <c r="B101" s="14"/>
-      <c r="C101" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E101" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F101" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="14"/>
       <c r="B102" s="14"/>
-      <c r="C102" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E102" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F102" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="14"/>
       <c r="B103" s="14"/>
-      <c r="C103" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E103" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F103" s="14">
-        <v>5.0000000000000001E-3</v>
-      </c>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>

<commit_message>
fix synthesis saver mode
</commit_message>
<xml_diff>
--- a/user_files/reagent_index.xlsx
+++ b/user_files/reagent_index.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xubar\OneDrive\Robot\Softwares\S2\user_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robot\S2-Software\user_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6048AC-430D-4C06-9B9B-A8BB4EC01C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="23233" windowHeight="12547"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reagent_index" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="142">
   <si>
     <t>CAS-NO</t>
   </si>
@@ -868,11 +869,15 @@
     <t>Pyran-4-amine</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>liquid1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1496,48 +1501,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1848,28 +1853,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:CG150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.1171875" style="38" customWidth="1"/>
-    <col min="2" max="2" width="13.76171875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="18.87890625" customWidth="1"/>
-    <col min="4" max="4" width="17.234375" customWidth="1"/>
-    <col min="5" max="5" width="15.1171875" customWidth="1"/>
-    <col min="6" max="6" width="31.41015625" customWidth="1"/>
-    <col min="7" max="7" width="10.3515625" customWidth="1"/>
+    <col min="1" max="1" width="35.125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="13.75" style="38" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="5" width="15.125" customWidth="1"/>
+    <col min="6" max="6" width="31.375" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" s="2" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:85" s="2" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
@@ -1972,7 +1977,7 @@
       <c r="CF1"/>
       <c r="CG1"/>
     </row>
-    <row r="2" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>66</v>
       </c>
@@ -2071,7 +2076,7 @@
       <c r="CF2"/>
       <c r="CG2"/>
     </row>
-    <row r="3" spans="1:85" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:85" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
         <v>64</v>
       </c>
@@ -2170,7 +2175,7 @@
       <c r="CF3"/>
       <c r="CG3"/>
     </row>
-    <row r="4" spans="1:85" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:85" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>92</v>
       </c>
@@ -2269,7 +2274,7 @@
       <c r="CF4"/>
       <c r="CG4"/>
     </row>
-    <row r="5" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
         <v>63</v>
       </c>
@@ -2368,7 +2373,7 @@
       <c r="CF5"/>
       <c r="CG5"/>
     </row>
-    <row r="6" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
         <v>65</v>
       </c>
@@ -2467,7 +2472,7 @@
       <c r="CF6"/>
       <c r="CG6"/>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A7" s="50" t="s">
         <v>94</v>
       </c>
@@ -2488,11 +2493,11 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8"/>
     </row>
-    <row r="9" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>96</v>
       </c>
@@ -2591,7 +2596,7 @@
       <c r="CF9" s="6"/>
       <c r="CG9" s="6"/>
     </row>
-    <row r="10" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>67</v>
       </c>
@@ -2690,7 +2695,7 @@
       <c r="CF10" s="6"/>
       <c r="CG10" s="6"/>
     </row>
-    <row r="11" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
@@ -2789,7 +2794,7 @@
       <c r="CF11" s="6"/>
       <c r="CG11" s="6"/>
     </row>
-    <row r="12" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>103</v>
       </c>
@@ -2888,7 +2893,7 @@
       <c r="CF12" s="6"/>
       <c r="CG12" s="6"/>
     </row>
-    <row r="13" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>48</v>
       </c>
@@ -2987,7 +2992,7 @@
       <c r="CF13" s="6"/>
       <c r="CG13" s="6"/>
     </row>
-    <row r="14" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:85" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
         <v>35</v>
       </c>
@@ -3086,11 +3091,11 @@
       <c r="CF14" s="6"/>
       <c r="CG14" s="6"/>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:85" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:85" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
         <v>108</v>
       </c>
@@ -3143,7 +3148,7 @@
       <c r="AL16"/>
       <c r="AM16"/>
     </row>
-    <row r="17" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
         <v>93</v>
       </c>
@@ -3196,7 +3201,7 @@
       <c r="AL17"/>
       <c r="AM17"/>
     </row>
-    <row r="18" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28"/>
       <c r="B18" s="27"/>
       <c r="C18" s="11" t="s">
@@ -3247,7 +3252,7 @@
       <c r="AL18"/>
       <c r="AM18"/>
     </row>
-    <row r="19" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28"/>
       <c r="B19" s="27"/>
       <c r="C19" s="11" t="s">
@@ -3298,7 +3303,7 @@
       <c r="AL19"/>
       <c r="AM19"/>
     </row>
-    <row r="20" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:39" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28"/>
       <c r="B20" s="27"/>
       <c r="C20" s="11" t="s">
@@ -3351,7 +3356,7 @@
       <c r="AL20"/>
       <c r="AM20"/>
     </row>
-    <row r="21" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:39" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
         <v>68</v>
       </c>
@@ -3406,11 +3411,11 @@
       <c r="AL21"/>
       <c r="AM21"/>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" s="37" t="s">
         <v>99</v>
       </c>
@@ -3433,7 +3438,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" s="37" t="s">
         <v>125</v>
       </c>
@@ -3456,7 +3461,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" s="37" t="s">
         <v>105</v>
       </c>
@@ -3479,7 +3484,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" s="37" t="s">
         <v>128</v>
       </c>
@@ -3502,7 +3507,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="52" t="s">
         <v>129</v>
       </c>
@@ -3525,7 +3530,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="54" t="s">
         <v>130</v>
       </c>
@@ -3548,7 +3553,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
         <v>132</v>
       </c>
@@ -3571,7 +3576,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="52"/>
       <c r="B30" s="52"/>
       <c r="C30" s="53" t="s">
@@ -3590,7 +3595,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="37" t="s">
         <v>138</v>
       </c>
@@ -3613,7 +3618,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" s="37"/>
       <c r="B32" s="37"/>
       <c r="C32" s="16" t="s">
@@ -3628,7 +3633,7 @@
       <c r="F32" s="13"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="37"/>
       <c r="B33" s="37"/>
       <c r="C33" s="16" t="s">
@@ -3647,8 +3652,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="37"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="37" t="s">
+        <v>141</v>
+      </c>
       <c r="B34" s="37"/>
       <c r="C34" s="16" t="s">
         <v>57</v>
@@ -3666,11 +3673,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35"/>
       <c r="B35"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="37" t="s">
         <v>140</v>
       </c>
@@ -3693,7 +3700,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="37" t="s">
         <v>135</v>
       </c>
@@ -3716,7 +3723,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="37" t="s">
         <v>122</v>
       </c>
@@ -3739,7 +3746,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="37"/>
       <c r="B39" s="37"/>
       <c r="C39" s="16" t="s">
@@ -3758,7 +3765,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="52" t="s">
         <v>113</v>
       </c>
@@ -3781,7 +3788,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="54" t="s">
         <v>119</v>
       </c>
@@ -3802,7 +3809,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="54" t="s">
         <v>115</v>
       </c>
@@ -3825,7 +3832,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="52" t="s">
         <v>117</v>
       </c>
@@ -3848,7 +3855,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="55" t="s">
         <v>121</v>
       </c>
@@ -3869,7 +3876,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="37" t="s">
         <v>107</v>
       </c>
@@ -3892,7 +3899,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="37"/>
       <c r="B46" s="37"/>
       <c r="C46" s="16" t="s">
@@ -3911,7 +3918,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="37" t="s">
         <v>137</v>
       </c>
@@ -3934,12 +3941,14 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="B48"/>
     </row>
-    <row r="49" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="29"/>
+    <row r="49" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="B49" s="30"/>
       <c r="C49" s="4" t="s">
         <v>37</v>
@@ -3989,7 +3998,7 @@
       <c r="AL49"/>
       <c r="AM49"/>
     </row>
-    <row r="50" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="29"/>
       <c r="B50" s="30"/>
       <c r="C50" s="4" t="s">
@@ -4040,7 +4049,7 @@
       <c r="AL50"/>
       <c r="AM50"/>
     </row>
-    <row r="51" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="29"/>
       <c r="B51" s="30"/>
       <c r="C51" s="4" t="s">
@@ -4091,7 +4100,7 @@
       <c r="AL51"/>
       <c r="AM51"/>
     </row>
-    <row r="52" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="29"/>
       <c r="B52" s="30"/>
       <c r="C52" s="4" t="s">
@@ -4142,10 +4151,8 @@
       <c r="AL52"/>
       <c r="AM52"/>
     </row>
-    <row r="53" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="29" t="s">
-        <v>54</v>
-      </c>
+    <row r="53" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="29"/>
       <c r="B53" s="30"/>
       <c r="C53" s="4" t="s">
         <v>7</v>
@@ -4195,7 +4202,7 @@
       <c r="AL53"/>
       <c r="AM53"/>
     </row>
-    <row r="54" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
       <c r="B54" s="30"/>
       <c r="C54" s="4" t="s">
@@ -4246,7 +4253,7 @@
       <c r="AL54"/>
       <c r="AM54"/>
     </row>
-    <row r="55" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="30" t="s">
         <v>46</v>
       </c>
@@ -4299,7 +4306,7 @@
       <c r="AL55"/>
       <c r="AM55"/>
     </row>
-    <row r="56" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="C56" s="4" t="s">
@@ -4350,7 +4357,7 @@
       <c r="AL56"/>
       <c r="AM56"/>
     </row>
-    <row r="57" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="30"/>
       <c r="B57" s="30"/>
       <c r="C57" s="4" t="s">
@@ -4401,7 +4408,7 @@
       <c r="AL57"/>
       <c r="AM57"/>
     </row>
-    <row r="58" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="30"/>
       <c r="B58" s="30"/>
       <c r="C58" s="4" t="s">
@@ -4452,7 +4459,7 @@
       <c r="AL58"/>
       <c r="AM58"/>
     </row>
-    <row r="59" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="30"/>
       <c r="B59" s="30"/>
       <c r="C59" s="4" t="s">
@@ -4503,7 +4510,7 @@
       <c r="AL59"/>
       <c r="AM59"/>
     </row>
-    <row r="60" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="30"/>
       <c r="B60" s="30"/>
       <c r="C60" s="4" t="s">
@@ -4554,7 +4561,7 @@
       <c r="AL60"/>
       <c r="AM60"/>
     </row>
-    <row r="61" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="30"/>
       <c r="B61" s="30"/>
       <c r="C61" s="4" t="s">
@@ -4605,7 +4612,7 @@
       <c r="AL61"/>
       <c r="AM61"/>
     </row>
-    <row r="62" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
       <c r="B62" s="30"/>
       <c r="C62" s="4" t="s">
@@ -4656,7 +4663,7 @@
       <c r="AL62"/>
       <c r="AM62"/>
     </row>
-    <row r="63" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
       <c r="B63" s="30"/>
       <c r="C63" s="4" t="s">
@@ -4707,7 +4714,7 @@
       <c r="AL63"/>
       <c r="AM63"/>
     </row>
-    <row r="64" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="30"/>
       <c r="B64" s="30"/>
       <c r="C64" s="4" t="s">
@@ -4758,7 +4765,7 @@
       <c r="AL64"/>
       <c r="AM64"/>
     </row>
-    <row r="65" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
       <c r="B65" s="30"/>
       <c r="C65" s="4" t="s">
@@ -4809,7 +4816,7 @@
       <c r="AL65"/>
       <c r="AM65"/>
     </row>
-    <row r="66" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="30"/>
       <c r="B66" s="30"/>
       <c r="C66" s="4" t="s">
@@ -4860,7 +4867,7 @@
       <c r="AL66"/>
       <c r="AM66"/>
     </row>
-    <row r="67" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
       <c r="B67" s="30"/>
       <c r="C67" s="4" t="s">
@@ -4911,7 +4918,7 @@
       <c r="AL67"/>
       <c r="AM67"/>
     </row>
-    <row r="68" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="30"/>
       <c r="B68" s="30"/>
       <c r="C68" s="4" t="s">
@@ -4962,7 +4969,7 @@
       <c r="AL68"/>
       <c r="AM68"/>
     </row>
-    <row r="69" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="30"/>
       <c r="B69" s="30"/>
       <c r="C69" s="4" t="s">
@@ -5013,7 +5020,7 @@
       <c r="AL69"/>
       <c r="AM69"/>
     </row>
-    <row r="70" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="30"/>
       <c r="B70" s="30"/>
       <c r="C70" s="4" t="s">
@@ -5064,7 +5071,7 @@
       <c r="AL70"/>
       <c r="AM70"/>
     </row>
-    <row r="71" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="30"/>
       <c r="B71" s="30"/>
       <c r="C71" s="4" t="s">
@@ -5115,7 +5122,7 @@
       <c r="AL71"/>
       <c r="AM71"/>
     </row>
-    <row r="72" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="30"/>
       <c r="B72" s="30"/>
       <c r="C72" s="4" t="s">
@@ -5166,7 +5173,7 @@
       <c r="AL72"/>
       <c r="AM72"/>
     </row>
-    <row r="73" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="30"/>
       <c r="B73" s="30"/>
       <c r="C73" s="4" t="s">
@@ -5217,7 +5224,7 @@
       <c r="AL73"/>
       <c r="AM73"/>
     </row>
-    <row r="74" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="30"/>
       <c r="B74" s="30"/>
       <c r="C74" s="4" t="s">
@@ -5268,7 +5275,7 @@
       <c r="AL74"/>
       <c r="AM74"/>
     </row>
-    <row r="75" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="30"/>
       <c r="B75" s="30"/>
       <c r="C75" s="4" t="s">
@@ -5319,7 +5326,7 @@
       <c r="AL75"/>
       <c r="AM75"/>
     </row>
-    <row r="76" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="29" t="s">
         <v>55</v>
       </c>
@@ -5372,11 +5379,11 @@
       <c r="AL76"/>
       <c r="AM76"/>
     </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A77"/>
       <c r="B77"/>
     </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A78" s="31" t="s">
         <v>73</v>
       </c>
@@ -5399,7 +5406,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A79" s="31" t="s">
         <v>74</v>
       </c>
@@ -5420,7 +5427,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A80" s="31" t="s">
         <v>75</v>
       </c>
@@ -5441,7 +5448,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="31"/>
       <c r="B81" s="33"/>
       <c r="C81" s="12" t="s">
@@ -5460,7 +5467,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="31"/>
       <c r="B82" s="33"/>
       <c r="C82" s="12" t="s">
@@ -5479,7 +5486,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="31"/>
       <c r="B83" s="33"/>
       <c r="C83" s="12" t="s">
@@ -5498,7 +5505,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="31"/>
       <c r="B84" s="33"/>
       <c r="C84" s="12" t="s">
@@ -5517,7 +5524,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="31"/>
       <c r="B85" s="33"/>
       <c r="C85" s="12" t="s">
@@ -5536,7 +5543,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="32" t="s">
         <v>76</v>
       </c>
@@ -5557,7 +5564,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="31" t="s">
         <v>77</v>
       </c>
@@ -5578,7 +5585,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="31" t="s">
         <v>78</v>
       </c>
@@ -5599,7 +5606,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="33"/>
       <c r="B89" s="33"/>
       <c r="C89" s="12" t="s">
@@ -5618,7 +5625,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="31" t="s">
         <v>60</v>
       </c>
@@ -5641,7 +5648,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="31" t="s">
         <v>79</v>
       </c>
@@ -5662,7 +5669,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="31" t="s">
         <v>80</v>
       </c>
@@ -5683,7 +5690,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="31" t="s">
         <v>81</v>
       </c>
@@ -5704,7 +5711,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="31" t="s">
         <v>82</v>
       </c>
@@ -5725,7 +5732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="31" t="s">
         <v>83</v>
       </c>
@@ -5746,7 +5753,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="31" t="s">
         <v>84</v>
       </c>
@@ -5767,7 +5774,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="33"/>
       <c r="B97" s="33"/>
       <c r="C97" s="12" t="s">
@@ -5786,7 +5793,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="31" t="s">
         <v>85</v>
       </c>
@@ -5807,7 +5814,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="33"/>
       <c r="B99" s="33"/>
       <c r="C99" s="12" t="s">
@@ -5826,7 +5833,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="31" t="s">
         <v>89</v>
       </c>
@@ -5847,7 +5854,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="31" t="s">
         <v>90</v>
       </c>
@@ -5868,7 +5875,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="31" t="s">
         <v>86</v>
       </c>
@@ -5889,7 +5896,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="33"/>
       <c r="B103" s="33"/>
       <c r="C103" s="12" t="s">
@@ -5908,7 +5915,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="31" t="s">
         <v>87</v>
       </c>
@@ -5929,7 +5936,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="31" t="s">
         <v>88</v>
       </c>
@@ -5950,11 +5957,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106"/>
       <c r="B106"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="34"/>
       <c r="B107" s="35"/>
       <c r="C107" s="18" t="s">
@@ -5973,7 +5980,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="34"/>
       <c r="B108" s="35"/>
       <c r="C108" s="18" t="s">
@@ -5992,7 +5999,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="34"/>
       <c r="B109" s="35"/>
       <c r="C109" s="18" t="s">
@@ -6011,7 +6018,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="35"/>
       <c r="B110" s="35"/>
       <c r="C110" s="18" t="s">
@@ -6030,7 +6037,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="35"/>
       <c r="B111" s="35"/>
       <c r="C111" s="18" t="s">
@@ -6049,7 +6056,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="35"/>
       <c r="B112" s="35"/>
       <c r="C112" s="18" t="s">
@@ -6068,7 +6075,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="35"/>
       <c r="B113" s="35"/>
       <c r="C113" s="18" t="s">
@@ -6087,7 +6094,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="35"/>
       <c r="B114" s="35"/>
       <c r="C114" s="18" t="s">
@@ -6106,7 +6113,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="35"/>
       <c r="B115" s="35"/>
       <c r="C115" s="18" t="s">
@@ -6125,7 +6132,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="35"/>
       <c r="B116" s="35"/>
       <c r="C116" s="18" t="s">
@@ -6144,7 +6151,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="35"/>
       <c r="B117" s="35"/>
       <c r="C117" s="18" t="s">
@@ -6163,7 +6170,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="35"/>
       <c r="B118" s="35"/>
       <c r="C118" s="18" t="s">
@@ -6182,7 +6189,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="35"/>
       <c r="B119" s="35"/>
       <c r="C119" s="18" t="s">
@@ -6201,7 +6208,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="35"/>
       <c r="B120" s="35"/>
       <c r="C120" s="18" t="s">
@@ -6220,7 +6227,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="35"/>
       <c r="B121" s="35"/>
       <c r="C121" s="18" t="s">
@@ -6239,7 +6246,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="35"/>
       <c r="B122" s="35"/>
       <c r="C122" s="18" t="s">
@@ -6258,7 +6265,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="35"/>
       <c r="B123" s="35"/>
       <c r="C123" s="18" t="s">
@@ -6277,7 +6284,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="35"/>
       <c r="B124" s="35"/>
       <c r="C124" s="18" t="s">
@@ -6296,7 +6303,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="35"/>
       <c r="B125" s="35"/>
       <c r="C125" s="18" t="s">
@@ -6315,7 +6322,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="35"/>
       <c r="B126" s="35"/>
       <c r="C126" s="18" t="s">
@@ -6334,7 +6341,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="35"/>
       <c r="B127" s="35"/>
       <c r="C127" s="18" t="s">
@@ -6353,7 +6360,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="35"/>
       <c r="B128" s="35"/>
       <c r="C128" s="18" t="s">
@@ -6372,7 +6379,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="35"/>
       <c r="B129" s="35"/>
       <c r="C129" s="18" t="s">
@@ -6391,7 +6398,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="35"/>
       <c r="B130" s="35"/>
       <c r="C130" s="18" t="s">
@@ -6410,7 +6417,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="35"/>
       <c r="B131" s="35"/>
       <c r="C131" s="18" t="s">
@@ -6429,7 +6436,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="35"/>
       <c r="B132" s="35"/>
       <c r="C132" s="18" t="s">
@@ -6448,7 +6455,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="35"/>
       <c r="B133" s="35"/>
       <c r="C133" s="18" t="s">
@@ -6467,7 +6474,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="35"/>
       <c r="B134" s="35"/>
       <c r="C134" s="18" t="s">
@@ -6486,7 +6493,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="135" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="40"/>
       <c r="B135" s="40"/>
       <c r="C135" s="41"/>
@@ -6497,7 +6504,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="36"/>
       <c r="B136" s="36"/>
       <c r="C136" s="13"/>
@@ -6508,7 +6515,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="36"/>
       <c r="B137" s="36"/>
       <c r="C137" s="13"/>
@@ -6519,7 +6526,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="36"/>
       <c r="B138" s="36"/>
       <c r="C138" s="13"/>
@@ -6530,7 +6537,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="36"/>
       <c r="B139" s="36"/>
       <c r="C139" s="13"/>
@@ -6541,7 +6548,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="36"/>
       <c r="B140" s="36"/>
       <c r="C140" s="13"/>
@@ -6552,7 +6559,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="36"/>
       <c r="B141" s="36"/>
       <c r="C141" s="13"/>
@@ -6563,7 +6570,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="36"/>
       <c r="B142" s="36"/>
       <c r="C142" s="13"/>
@@ -6574,7 +6581,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="36"/>
       <c r="B143" s="36"/>
       <c r="C143" s="13"/>
@@ -6585,7 +6592,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="36"/>
       <c r="B144" s="36"/>
       <c r="C144" s="13"/>
@@ -6596,7 +6603,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="36"/>
       <c r="B145" s="36"/>
       <c r="C145" s="13"/>
@@ -6607,7 +6614,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="36"/>
       <c r="B146" s="36"/>
       <c r="C146" s="13"/>
@@ -6618,7 +6625,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="36"/>
       <c r="B147" s="36"/>
       <c r="C147" s="13"/>
@@ -6629,7 +6636,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="36"/>
       <c r="B148" s="36"/>
       <c r="C148" s="13"/>
@@ -6640,7 +6647,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="36"/>
       <c r="B149" s="36"/>
       <c r="C149" s="13"/>
@@ -6651,7 +6658,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="36"/>
       <c r="B150" s="36"/>
       <c r="C150" s="13"/>
@@ -6670,12 +6677,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>